<commit_message>
Saving trace into EventLog
</commit_message>
<xml_diff>
--- a/Docs/Portfolio-DataDomain.xlsx
+++ b/Docs/Portfolio-DataDomain.xlsx
@@ -5,21 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aborj\Documents\OzoraSoft\Portfolio\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aborj\Documents\GitHub\OzoraSoft-Portfolio\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2FA064-9D8F-42E8-832B-EA7343BCD1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3340DBE-D584-4DC9-848B-7F1FF389E342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26955" yWindow="1305" windowWidth="21765" windowHeight="13335" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21300" yWindow="795" windowWidth="16470" windowHeight="13335" tabRatio="744" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Entities" sheetId="1" r:id="rId1"/>
-    <sheet name="Enums" sheetId="2" r:id="rId2"/>
-    <sheet name="Tables" sheetId="4" r:id="rId3"/>
-    <sheet name="Abbreviatures" sheetId="5" r:id="rId4"/>
+    <sheet name="infoseccontrols-Entities" sheetId="1" r:id="rId1"/>
+    <sheet name="infoseccontrols-Enums" sheetId="2" r:id="rId2"/>
+    <sheet name="infoseccontrols-Tables" sheetId="4" r:id="rId3"/>
+    <sheet name="infoseccontrolsAbbreviatures" sheetId="5" r:id="rId4"/>
+    <sheet name="shared-Enums" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Enums!$A$1:$B$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'infoseccontrols-Enums'!$A$1:$B$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'shared-Enums'!$A$1:$B$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="401">
   <si>
     <t>Entity</t>
   </si>
@@ -1145,6 +1147,97 @@
   </si>
   <si>
     <t>Asset.Supporting</t>
+  </si>
+  <si>
+    <t>EventLog.Projects</t>
+  </si>
+  <si>
+    <t>EventLog.Modules</t>
+  </si>
+  <si>
+    <t>EventLog.Actions</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>OzoraSoft.API.Services</t>
+  </si>
+  <si>
+    <t>OzoraSoft.API.Utils</t>
+  </si>
+  <si>
+    <t>OzoraSoft.AppHost</t>
+  </si>
+  <si>
+    <t>OzoraSoft.Tests</t>
+  </si>
+  <si>
+    <t>OzoraSoft.Console</t>
+  </si>
+  <si>
+    <t>OzoraSoft.Web</t>
+  </si>
+  <si>
+    <t>OzoraSoft.Library.Enums</t>
+  </si>
+  <si>
+    <t>OzoraSoft.Library.Messaging</t>
+  </si>
+  <si>
+    <t>OzoraSoft.Library.PictureMaker</t>
+  </si>
+  <si>
+    <t>OzoraSoft.Library.Security</t>
+  </si>
+  <si>
+    <t>OzoraSoft.ServiceDefaults</t>
+  </si>
+  <si>
+    <t>Shared</t>
+  </si>
+  <si>
+    <t>InfoSecControls</t>
+  </si>
+  <si>
+    <t>PictureMaker</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Utils.Authentication</t>
+  </si>
+  <si>
+    <t>Utils.Messaging</t>
+  </si>
+  <si>
+    <t>EventLog.Controllers</t>
+  </si>
+  <si>
+    <t>InfoSecControls.SystemParameters</t>
+  </si>
+  <si>
+    <t>InfoSecControls.OrganizationPolicies</t>
+  </si>
+  <si>
+    <t>Shared.EventLogs</t>
+  </si>
+  <si>
+    <t>INSERT INTO asjrf517_ozorasoft_shared.SystemParameters
+(group_id, id, name, active) VALUES</t>
   </si>
 </sst>
 </file>
@@ -1850,11 +1943,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2991,7 +3084,7 @@
         <v>68</v>
       </c>
       <c r="E3" s="18">
-        <f>VLOOKUP(D3,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D3,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F3" s="25" t="s">
@@ -3031,7 +3124,7 @@
         <v>68</v>
       </c>
       <c r="E4" s="18">
-        <f>VLOOKUP(D4,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D4,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F4" s="25" t="s">
@@ -3071,7 +3164,7 @@
         <v>68</v>
       </c>
       <c r="E5" s="18">
-        <f>VLOOKUP(D5,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D5,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F5" s="25" t="s">
@@ -3111,7 +3204,7 @@
         <v>68</v>
       </c>
       <c r="E6" s="18">
-        <f>VLOOKUP(D6,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D6,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F6" s="25" t="s">
@@ -3151,7 +3244,7 @@
         <v>68</v>
       </c>
       <c r="E7" s="18">
-        <f>VLOOKUP(D7,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D7,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F7" s="25" t="s">
@@ -3191,7 +3284,7 @@
         <v>68</v>
       </c>
       <c r="E8" s="18">
-        <f>VLOOKUP(D8,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D8,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F8" s="25" t="s">
@@ -3231,7 +3324,7 @@
         <v>68</v>
       </c>
       <c r="E9" s="18">
-        <f>VLOOKUP(D9,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D9,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F9" s="25" t="s">
@@ -3271,7 +3364,7 @@
         <v>68</v>
       </c>
       <c r="E10" s="18">
-        <f>VLOOKUP(D10,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D10,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F10" s="25" t="s">
@@ -3311,7 +3404,7 @@
         <v>68</v>
       </c>
       <c r="E11" s="18">
-        <f>VLOOKUP(D11,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D11,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F11" s="25" t="s">
@@ -3351,7 +3444,7 @@
         <v>68</v>
       </c>
       <c r="E12" s="18">
-        <f>VLOOKUP(D12,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D12,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F12" s="25" t="s">
@@ -3391,7 +3484,7 @@
         <v>68</v>
       </c>
       <c r="E13" s="18">
-        <f>VLOOKUP(D13,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D13,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F13" s="25" t="s">
@@ -3431,7 +3524,7 @@
         <v>68</v>
       </c>
       <c r="E14" s="18">
-        <f>VLOOKUP(D14,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D14,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F14" s="25" t="s">
@@ -3471,7 +3564,7 @@
         <v>68</v>
       </c>
       <c r="E15" s="18">
-        <f>VLOOKUP(D15,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D15,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F15" s="25" t="s">
@@ -3511,7 +3604,7 @@
         <v>68</v>
       </c>
       <c r="E16" s="18">
-        <f>VLOOKUP(D16,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D16,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F16" s="25" t="s">
@@ -3551,7 +3644,7 @@
         <v>68</v>
       </c>
       <c r="E17" s="18">
-        <f>VLOOKUP(D17,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D17,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F17" s="25" t="s">
@@ -3591,7 +3684,7 @@
         <v>68</v>
       </c>
       <c r="E18" s="18">
-        <f>VLOOKUP(D18,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D18,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F18" s="25" t="s">
@@ -3631,7 +3724,7 @@
         <v>68</v>
       </c>
       <c r="E19" s="18">
-        <f>VLOOKUP(D19,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D19,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F19" s="25" t="s">
@@ -3671,7 +3764,7 @@
         <v>68</v>
       </c>
       <c r="E20" s="18">
-        <f>VLOOKUP(D20,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D20,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F20" s="25" t="s">
@@ -3711,7 +3804,7 @@
         <v>68</v>
       </c>
       <c r="E21" s="18">
-        <f>VLOOKUP(D21,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D21,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F21" s="25" t="s">
@@ -3751,7 +3844,7 @@
         <v>68</v>
       </c>
       <c r="E22" s="18">
-        <f>VLOOKUP(D22,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D22,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F22" s="25" t="s">
@@ -3791,7 +3884,7 @@
         <v>68</v>
       </c>
       <c r="E23" s="18">
-        <f>VLOOKUP(D23,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D23,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F23" s="25" t="s">
@@ -3831,7 +3924,7 @@
         <v>68</v>
       </c>
       <c r="E24" s="18">
-        <f>VLOOKUP(D24,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D24,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F24" s="25" t="s">
@@ -3871,7 +3964,7 @@
         <v>68</v>
       </c>
       <c r="E25" s="18">
-        <f>VLOOKUP(D25,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D25,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F25" s="25" t="s">
@@ -3911,7 +4004,7 @@
         <v>68</v>
       </c>
       <c r="E26" s="18">
-        <f>VLOOKUP(D26,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D26,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F26" s="25" t="s">
@@ -3951,7 +4044,7 @@
         <v>68</v>
       </c>
       <c r="E27" s="18">
-        <f>VLOOKUP(D27,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D27,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F27" s="25" t="s">
@@ -3991,7 +4084,7 @@
         <v>68</v>
       </c>
       <c r="E28" s="18">
-        <f>VLOOKUP(D28,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D28,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F28" s="25" t="s">
@@ -4031,7 +4124,7 @@
         <v>68</v>
       </c>
       <c r="E29" s="18">
-        <f>VLOOKUP(D29,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D29,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F29" s="25" t="s">
@@ -4071,7 +4164,7 @@
         <v>68</v>
       </c>
       <c r="E30" s="18">
-        <f>VLOOKUP(D30,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D30,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F30" s="25" t="s">
@@ -4111,7 +4204,7 @@
         <v>68</v>
       </c>
       <c r="E31" s="18">
-        <f>VLOOKUP(D31,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D31,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F31" s="25" t="s">
@@ -4151,7 +4244,7 @@
         <v>68</v>
       </c>
       <c r="E32" s="18">
-        <f>VLOOKUP(D32,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D32,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F32" s="25" t="s">
@@ -4191,7 +4284,7 @@
         <v>68</v>
       </c>
       <c r="E33" s="18">
-        <f>VLOOKUP(D33,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D33,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F33" s="25" t="s">
@@ -4231,7 +4324,7 @@
         <v>68</v>
       </c>
       <c r="E34" s="18">
-        <f>VLOOKUP(D34,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D34,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F34" s="25" t="s">
@@ -4271,7 +4364,7 @@
         <v>68</v>
       </c>
       <c r="E35" s="18">
-        <f>VLOOKUP(D35,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D35,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F35" s="25" t="s">
@@ -4311,7 +4404,7 @@
         <v>68</v>
       </c>
       <c r="E36" s="18">
-        <f>VLOOKUP(D36,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D36,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F36" s="25" t="s">
@@ -4351,7 +4444,7 @@
         <v>68</v>
       </c>
       <c r="E37" s="18">
-        <f>VLOOKUP(D37,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D37,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F37" s="25" t="s">
@@ -4391,7 +4484,7 @@
         <v>68</v>
       </c>
       <c r="E38" s="18">
-        <f>VLOOKUP(D38,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D38,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F38" s="25" t="s">
@@ -4431,7 +4524,7 @@
         <v>68</v>
       </c>
       <c r="E39" s="18">
-        <f>VLOOKUP(D39,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D39,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="F39" s="25" t="s">
@@ -4471,7 +4564,7 @@
         <v>69</v>
       </c>
       <c r="E40" s="18">
-        <f>VLOOKUP(D40,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D40,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>12</v>
       </c>
       <c r="F40" s="25" t="s">
@@ -4511,7 +4604,7 @@
         <v>69</v>
       </c>
       <c r="E41" s="18">
-        <f>VLOOKUP(D41,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D41,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>12</v>
       </c>
       <c r="F41" s="25" t="s">
@@ -4551,7 +4644,7 @@
         <v>69</v>
       </c>
       <c r="E42" s="18">
-        <f>VLOOKUP(D42,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D42,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>12</v>
       </c>
       <c r="F42" s="25" t="s">
@@ -4591,7 +4684,7 @@
         <v>69</v>
       </c>
       <c r="E43" s="18">
-        <f>VLOOKUP(D43,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D43,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>12</v>
       </c>
       <c r="F43" s="25" t="s">
@@ -4631,7 +4724,7 @@
         <v>69</v>
       </c>
       <c r="E44" s="18">
-        <f>VLOOKUP(D44,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D44,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>12</v>
       </c>
       <c r="F44" s="25" t="s">
@@ -4671,7 +4764,7 @@
         <v>69</v>
       </c>
       <c r="E45" s="18">
-        <f>VLOOKUP(D45,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D45,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>12</v>
       </c>
       <c r="F45" s="25" t="s">
@@ -4711,7 +4804,7 @@
         <v>69</v>
       </c>
       <c r="E46" s="18">
-        <f>VLOOKUP(D46,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D46,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>12</v>
       </c>
       <c r="F46" s="25" t="s">
@@ -4751,7 +4844,7 @@
         <v>69</v>
       </c>
       <c r="E47" s="18">
-        <f>VLOOKUP(D47,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D47,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>12</v>
       </c>
       <c r="F47" s="25" t="s">
@@ -4791,7 +4884,7 @@
         <v>70</v>
       </c>
       <c r="E48" s="18">
-        <f>VLOOKUP(D48,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D48,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F48" s="25" t="s">
@@ -4831,7 +4924,7 @@
         <v>70</v>
       </c>
       <c r="E49" s="18">
-        <f>VLOOKUP(D49,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D49,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F49" s="25" t="s">
@@ -4871,7 +4964,7 @@
         <v>70</v>
       </c>
       <c r="E50" s="18">
-        <f>VLOOKUP(D50,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D50,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F50" s="25" t="s">
@@ -4911,7 +5004,7 @@
         <v>70</v>
       </c>
       <c r="E51" s="18">
-        <f>VLOOKUP(D51,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D51,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F51" s="25" t="s">
@@ -4951,7 +5044,7 @@
         <v>70</v>
       </c>
       <c r="E52" s="18">
-        <f>VLOOKUP(D52,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D52,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F52" s="25" t="s">
@@ -4991,7 +5084,7 @@
         <v>70</v>
       </c>
       <c r="E53" s="18">
-        <f>VLOOKUP(D53,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D53,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F53" s="25" t="s">
@@ -5031,7 +5124,7 @@
         <v>70</v>
       </c>
       <c r="E54" s="18">
-        <f>VLOOKUP(D54,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D54,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F54" s="25" t="s">
@@ -5071,7 +5164,7 @@
         <v>70</v>
       </c>
       <c r="E55" s="18">
-        <f>VLOOKUP(D55,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D55,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F55" s="25" t="s">
@@ -5111,7 +5204,7 @@
         <v>70</v>
       </c>
       <c r="E56" s="18">
-        <f>VLOOKUP(D56,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D56,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F56" s="25" t="s">
@@ -5151,7 +5244,7 @@
         <v>70</v>
       </c>
       <c r="E57" s="18">
-        <f>VLOOKUP(D57,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D57,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F57" s="25" t="s">
@@ -5191,7 +5284,7 @@
         <v>70</v>
       </c>
       <c r="E58" s="18">
-        <f>VLOOKUP(D58,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D58,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F58" s="25" t="s">
@@ -5231,7 +5324,7 @@
         <v>70</v>
       </c>
       <c r="E59" s="18">
-        <f>VLOOKUP(D59,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D59,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F59" s="25" t="s">
@@ -5271,7 +5364,7 @@
         <v>70</v>
       </c>
       <c r="E60" s="18">
-        <f>VLOOKUP(D60,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D60,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F60" s="25" t="s">
@@ -5311,7 +5404,7 @@
         <v>70</v>
       </c>
       <c r="E61" s="18">
-        <f>VLOOKUP(D61,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D61,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F61" s="25" t="s">
@@ -5351,7 +5444,7 @@
         <v>71</v>
       </c>
       <c r="E62" s="18">
-        <f>VLOOKUP(D62,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D62,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F62" s="25" t="s">
@@ -5391,7 +5484,7 @@
         <v>71</v>
       </c>
       <c r="E63" s="18">
-        <f>VLOOKUP(D63,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D63,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F63" s="25" t="s">
@@ -5431,7 +5524,7 @@
         <v>71</v>
       </c>
       <c r="E64" s="18">
-        <f>VLOOKUP(D64,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D64,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F64" s="25" t="s">
@@ -5471,7 +5564,7 @@
         <v>71</v>
       </c>
       <c r="E65" s="18">
-        <f>VLOOKUP(D65,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D65,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F65" s="25" t="s">
@@ -5511,7 +5604,7 @@
         <v>71</v>
       </c>
       <c r="E66" s="18">
-        <f>VLOOKUP(D66,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D66,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F66" s="25" t="s">
@@ -5551,7 +5644,7 @@
         <v>71</v>
       </c>
       <c r="E67" s="18">
-        <f>VLOOKUP(D67,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D67,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F67" s="25" t="s">
@@ -5591,7 +5684,7 @@
         <v>71</v>
       </c>
       <c r="E68" s="18">
-        <f>VLOOKUP(D68,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D68,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F68" s="25" t="s">
@@ -5631,7 +5724,7 @@
         <v>71</v>
       </c>
       <c r="E69" s="18">
-        <f>VLOOKUP(D69,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D69,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F69" s="25" t="s">
@@ -5671,7 +5764,7 @@
         <v>71</v>
       </c>
       <c r="E70" s="18">
-        <f>VLOOKUP(D70,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D70,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F70" s="25" t="s">
@@ -5711,7 +5804,7 @@
         <v>71</v>
       </c>
       <c r="E71" s="18">
-        <f>VLOOKUP(D71,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D71,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F71" s="25" t="s">
@@ -5751,7 +5844,7 @@
         <v>71</v>
       </c>
       <c r="E72" s="18">
-        <f>VLOOKUP(D72,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D72,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F72" s="25" t="s">
@@ -5791,7 +5884,7 @@
         <v>71</v>
       </c>
       <c r="E73" s="18">
-        <f>VLOOKUP(D73,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D73,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F73" s="25" t="s">
@@ -5831,7 +5924,7 @@
         <v>71</v>
       </c>
       <c r="E74" s="18">
-        <f>VLOOKUP(D74,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D74,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F74" s="25" t="s">
@@ -5871,7 +5964,7 @@
         <v>71</v>
       </c>
       <c r="E75" s="18">
-        <f>VLOOKUP(D75,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D75,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F75" s="25" t="s">
@@ -5911,7 +6004,7 @@
         <v>71</v>
       </c>
       <c r="E76" s="18">
-        <f>VLOOKUP(D76,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D76,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F76" s="25" t="s">
@@ -5951,7 +6044,7 @@
         <v>71</v>
       </c>
       <c r="E77" s="18">
-        <f>VLOOKUP(D77,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D77,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F77" s="25" t="s">
@@ -5991,7 +6084,7 @@
         <v>71</v>
       </c>
       <c r="E78" s="18">
-        <f>VLOOKUP(D78,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D78,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F78" s="25" t="s">
@@ -6031,7 +6124,7 @@
         <v>71</v>
       </c>
       <c r="E79" s="18">
-        <f>VLOOKUP(D79,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D79,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F79" s="25" t="s">
@@ -6071,7 +6164,7 @@
         <v>71</v>
       </c>
       <c r="E80" s="18">
-        <f>VLOOKUP(D80,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D80,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F80" s="25" t="s">
@@ -6111,7 +6204,7 @@
         <v>71</v>
       </c>
       <c r="E81" s="18">
-        <f>VLOOKUP(D81,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D81,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F81" s="25" t="s">
@@ -6151,7 +6244,7 @@
         <v>71</v>
       </c>
       <c r="E82" s="18">
-        <f>VLOOKUP(D82,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D82,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F82" s="25" t="s">
@@ -6191,7 +6284,7 @@
         <v>71</v>
       </c>
       <c r="E83" s="18">
-        <f>VLOOKUP(D83,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D83,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F83" s="25" t="s">
@@ -6231,7 +6324,7 @@
         <v>71</v>
       </c>
       <c r="E84" s="18">
-        <f>VLOOKUP(D84,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D84,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F84" s="25" t="s">
@@ -6271,7 +6364,7 @@
         <v>71</v>
       </c>
       <c r="E85" s="18">
-        <f>VLOOKUP(D85,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D85,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F85" s="25" t="s">
@@ -6311,7 +6404,7 @@
         <v>71</v>
       </c>
       <c r="E86" s="18">
-        <f>VLOOKUP(D86,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D86,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F86" s="25" t="s">
@@ -6351,7 +6444,7 @@
         <v>71</v>
       </c>
       <c r="E87" s="18">
-        <f>VLOOKUP(D87,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D87,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F87" s="25" t="s">
@@ -6391,7 +6484,7 @@
         <v>71</v>
       </c>
       <c r="E88" s="18">
-        <f>VLOOKUP(D88,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D88,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F88" s="25" t="s">
@@ -6431,7 +6524,7 @@
         <v>71</v>
       </c>
       <c r="E89" s="18">
-        <f>VLOOKUP(D89,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D89,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F89" s="25" t="s">
@@ -6471,7 +6564,7 @@
         <v>71</v>
       </c>
       <c r="E90" s="18">
-        <f>VLOOKUP(D90,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D90,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F90" s="25" t="s">
@@ -6511,7 +6604,7 @@
         <v>71</v>
       </c>
       <c r="E91" s="18">
-        <f>VLOOKUP(D91,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D91,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F91" s="25" t="s">
@@ -6551,7 +6644,7 @@
         <v>71</v>
       </c>
       <c r="E92" s="18">
-        <f>VLOOKUP(D92,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D92,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F92" s="25" t="s">
@@ -6591,7 +6684,7 @@
         <v>71</v>
       </c>
       <c r="E93" s="18">
-        <f>VLOOKUP(D93,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D93,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F93" s="25" t="s">
@@ -6631,7 +6724,7 @@
         <v>71</v>
       </c>
       <c r="E94" s="18">
-        <f>VLOOKUP(D94,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D94,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F94" s="25" t="s">
@@ -6671,7 +6764,7 @@
         <v>71</v>
       </c>
       <c r="E95" s="18">
-        <f>VLOOKUP(D95,Enums!$B$2:$C$55, 2,FALSE)</f>
+        <f>VLOOKUP(D95,'infoseccontrols-Enums'!$B$2:$C$55, 2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="F95" s="25" t="s">
@@ -6952,4 +7045,593 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB216624-9E4C-4390-839B-FA06F79CDE80}">
+  <dimension ref="A1:F30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="12"/>
+    <col min="6" max="6" width="79.7109375" style="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="C2" s="8">
+        <v>10</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="F2" s="20" t="str">
+        <f t="shared" ref="F2:F29" si="0">_xlfn.CONCAT("(",A2,", ",C2, ", '", B2, "', b'",D2,"'),")</f>
+        <v>(0, 10, 'EventLog.Projects', b'1'),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="F3" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(10, 1, 'OzoraSoft.API.Services', b'1'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="C4" s="8">
+        <f t="shared" ref="C4:C30" si="1">C3+1</f>
+        <v>2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="F4" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(10, 2, 'OzoraSoft.API.Utils', b'1'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C5" s="8">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="F5" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(10, 3, 'OzoraSoft.Console', b'1'),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="C6" s="8">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(10, 4, 'OzoraSoft.Tests', b'1'),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C7" s="8">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1</v>
+      </c>
+      <c r="F7" s="20" t="str">
+        <f t="shared" ref="F7:F11" si="2">_xlfn.CONCAT("(",A7,", ",C7, ", '", B7, "', b'",D7,"'),")</f>
+        <v>(10, 5, 'OzoraSoft.AppHost', b'1'),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C8" s="8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="20" t="str">
+        <f>_xlfn.CONCAT("(",A8,", ",C8, ", '", B8, "', b'",D8,"'),")</f>
+        <v>(10, 6, 'OzoraSoft.ServiceDefaults', b'1'),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="C9" s="8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="F9" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>(10, 7, 'OzoraSoft.Web', b'1'),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="C10" s="8">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>(10, 8, 'OzoraSoft.Library.Enums', b'1'),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="C11" s="8">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1</v>
+      </c>
+      <c r="F11" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>(10, 9, 'OzoraSoft.Library.Messaging', b'1'),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C12" s="8">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1</v>
+      </c>
+      <c r="F12" s="20" t="str">
+        <f t="shared" ref="F12:F13" si="3">_xlfn.CONCAT("(",A12,", ",C12, ", '", B12, "', b'",D12,"'),")</f>
+        <v>(10, 10, 'OzoraSoft.Library.PictureMaker', b'1'),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C13" s="8">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>(10, 11, 'OzoraSoft.Library.Security', b'1'),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>0</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="C14" s="8">
+        <v>20</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
+      <c r="F14" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(0, 20, 'EventLog.Modules', b'1'),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <f>A6+10</f>
+        <v>20</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
+      <c r="F15" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(20, 1, 'Shared', b'1'),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>20</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="C16" s="8">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="F16" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(20, 2, 'Security', b'1'),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>20</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="C17" s="8">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="F17" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(20, 3, 'InfoSecControls', b'1'),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>20</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="C18" s="8">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
+      <c r="F18" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(20, 4, 'PictureMaker', b'1'),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>0</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="C19" s="8">
+        <v>30</v>
+      </c>
+      <c r="D19" s="8">
+        <v>1</v>
+      </c>
+      <c r="F19" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(0, 30, 'EventLog.Controllers', b'1'),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <f>A18+10</f>
+        <v>30</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1</v>
+      </c>
+      <c r="F20" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(30, 1, 'Utils.Authentication', b'1'),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>30</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C21" s="8">
+        <f>C20+1</f>
+        <v>2</v>
+      </c>
+      <c r="D21" s="8">
+        <v>1</v>
+      </c>
+      <c r="F21" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(30, 2, 'Utils.Messaging', b'1'),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>30</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C22" s="8">
+        <f t="shared" ref="C22:C24" si="4">C21+1</f>
+        <v>3</v>
+      </c>
+      <c r="D22" s="8">
+        <v>1</v>
+      </c>
+      <c r="F22" s="20" t="str">
+        <f t="shared" ref="F22" si="5">_xlfn.CONCAT("(",A22,", ",C22, ", '", B22, "', b'",D22,"'),")</f>
+        <v>(30, 3, 'Shared.EventLogs', b'1'),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>30</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C23" s="8">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="D23" s="8">
+        <v>1</v>
+      </c>
+      <c r="F23" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(30, 4, 'InfoSecControls.SystemParameters', b'1'),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>30</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="C24" s="8">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="D24" s="8">
+        <v>1</v>
+      </c>
+      <c r="F24" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(30, 5, 'InfoSecControls.OrganizationPolicies', b'1'),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>0</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="C25" s="8">
+        <v>40</v>
+      </c>
+      <c r="D25" s="8">
+        <v>1</v>
+      </c>
+      <c r="F25" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(0, 40, 'EventLog.Actions', b'1'),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <f>A24+10</f>
+        <v>40</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C26" s="8">
+        <v>1</v>
+      </c>
+      <c r="D26" s="8">
+        <v>1</v>
+      </c>
+      <c r="F26" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(40, 1, 'Create', b'1'),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
+        <v>40</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="C27" s="8">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D27" s="8">
+        <v>1</v>
+      </c>
+      <c r="F27" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(40, 2, 'Read', b'1'),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <v>40</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="C28" s="8">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D28" s="8">
+        <v>1</v>
+      </c>
+      <c r="F28" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(40, 3, 'Update', b'1'),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
+        <v>40</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C29" s="8">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D29" s="8">
+        <v>1</v>
+      </c>
+      <c r="F29" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>(40, 4, 'Delete', b'1'),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>40</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="C30" s="8">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D30" s="8">
+        <v>1</v>
+      </c>
+      <c r="F30" s="20" t="str">
+        <f t="shared" ref="F30" si="6">_xlfn.CONCAT("(",A30,", ",C30, ", '", B30, "', b'",D30,"'),")</f>
+        <v>(40, 5, 'List', b'1'),</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B29" xr:uid="{AD08FBCA-206E-41A1-8589-5F1F7EE43364}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add VideoCapture API [#5]
</commit_message>
<xml_diff>
--- a/Docs/Portfolio-DataDomain.xlsx
+++ b/Docs/Portfolio-DataDomain.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aborj\Documents\GitHub\OzoraSoft-Portfolio\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB26F392-E4AE-4A55-88B4-B25D02F2136E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B4E3B6-5406-40D2-8575-FF2D3D54E901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21300" yWindow="795" windowWidth="16470" windowHeight="13335" tabRatio="744" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="744" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="infoseccontrols-Entities" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'infoseccontrols-Enums'!$A$1:$B$55</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'shared-Enums'!$A$1:$B$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'shared-Enums'!$A$1:$B$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="403">
   <si>
     <t>Entity</t>
   </si>
@@ -1236,15 +1236,20 @@
     <t>Shared.EventLogs</t>
   </si>
   <si>
-    <t>INSERT INTO asjrf517_ozorasoft_shared.SystemParameters
-(group_id, id, name, active) VALUES</t>
+    <t>Transit</t>
+  </si>
+  <si>
+    <t>Tranist.RealTimeStream</t>
+  </si>
+  <si>
+    <t>[!] Update enmEventLog</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1292,6 +1297,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1383,7 +1396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1440,6 +1453,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7049,13 +7063,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB216624-9E4C-4390-839B-FA06F79CDE80}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7064,10 +7078,9 @@
     <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="12"/>
-    <col min="6" max="6" width="79.7109375" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>125</v>
       </c>
@@ -7080,8 +7093,8 @@
       <c r="D1" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="F1" s="19" t="s">
-        <v>400</v>
+      <c r="F1" s="28" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7097,10 +7110,6 @@
       <c r="D2" s="8">
         <v>1</v>
       </c>
-      <c r="F2" s="20" t="str">
-        <f t="shared" ref="F2:F29" si="0">_xlfn.CONCAT("(",A2,", ",C2, ", '", B2, "', b'",D2,"'),")</f>
-        <v>(0, 10, 'EventLog.Projects', b'1'),</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -7115,10 +7124,6 @@
       <c r="D3" s="8">
         <v>1</v>
       </c>
-      <c r="F3" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(10, 1, 'OzoraSoft.API.Services', b'1'),</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
@@ -7128,15 +7133,11 @@
         <v>380</v>
       </c>
       <c r="C4" s="8">
-        <f t="shared" ref="C4:C30" si="1">C3+1</f>
+        <f t="shared" ref="C4:C32" si="0">C3+1</f>
         <v>2</v>
       </c>
       <c r="D4" s="8">
         <v>1</v>
-      </c>
-      <c r="F4" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(10, 2, 'OzoraSoft.API.Utils', b'1'),</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -7147,15 +7148,11 @@
         <v>383</v>
       </c>
       <c r="C5" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D5" s="8">
         <v>1</v>
-      </c>
-      <c r="F5" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(10, 3, 'OzoraSoft.Console', b'1'),</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -7166,15 +7163,11 @@
         <v>382</v>
       </c>
       <c r="C6" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D6" s="8">
         <v>1</v>
-      </c>
-      <c r="F6" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(10, 4, 'OzoraSoft.Tests', b'1'),</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -7185,15 +7178,11 @@
         <v>381</v>
       </c>
       <c r="C7" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D7" s="8">
         <v>1</v>
-      </c>
-      <c r="F7" s="20" t="str">
-        <f t="shared" ref="F7:F11" si="2">_xlfn.CONCAT("(",A7,", ",C7, ", '", B7, "', b'",D7,"'),")</f>
-        <v>(10, 5, 'OzoraSoft.AppHost', b'1'),</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -7204,15 +7193,11 @@
         <v>389</v>
       </c>
       <c r="C8" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D8" s="8">
         <v>1</v>
-      </c>
-      <c r="F8" s="20" t="str">
-        <f>_xlfn.CONCAT("(",A8,", ",C8, ", '", B8, "', b'",D8,"'),")</f>
-        <v>(10, 6, 'OzoraSoft.ServiceDefaults', b'1'),</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -7223,15 +7208,11 @@
         <v>384</v>
       </c>
       <c r="C9" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="D9" s="8">
         <v>1</v>
-      </c>
-      <c r="F9" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v>(10, 7, 'OzoraSoft.Web', b'1'),</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -7242,15 +7223,11 @@
         <v>385</v>
       </c>
       <c r="C10" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D10" s="8">
         <v>1</v>
-      </c>
-      <c r="F10" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v>(10, 8, 'OzoraSoft.Library.Enums', b'1'),</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -7261,15 +7238,11 @@
         <v>386</v>
       </c>
       <c r="C11" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="D11" s="8">
         <v>1</v>
-      </c>
-      <c r="F11" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v>(10, 9, 'OzoraSoft.Library.Messaging', b'1'),</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -7280,15 +7253,11 @@
         <v>387</v>
       </c>
       <c r="C12" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="D12" s="8">
         <v>1</v>
-      </c>
-      <c r="F12" s="20" t="str">
-        <f t="shared" ref="F12:F13" si="3">_xlfn.CONCAT("(",A12,", ",C12, ", '", B12, "', b'",D12,"'),")</f>
-        <v>(10, 10, 'OzoraSoft.Library.PictureMaker', b'1'),</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -7299,15 +7268,11 @@
         <v>388</v>
       </c>
       <c r="C13" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="D13" s="8">
         <v>1</v>
-      </c>
-      <c r="F13" s="20" t="str">
-        <f t="shared" si="3"/>
-        <v>(10, 11, 'OzoraSoft.Library.Security', b'1'),</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7322,10 +7287,6 @@
       </c>
       <c r="D14" s="8">
         <v>1</v>
-      </c>
-      <c r="F14" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(0, 20, 'EventLog.Modules', b'1'),</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -7342,10 +7303,6 @@
       <c r="D15" s="8">
         <v>1</v>
       </c>
-      <c r="F15" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(20, 1, 'Shared', b'1'),</v>
-      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
@@ -7355,18 +7312,14 @@
         <v>393</v>
       </c>
       <c r="C16" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D16" s="8">
         <v>1</v>
       </c>
-      <c r="F16" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(20, 2, 'Security', b'1'),</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>20</v>
       </c>
@@ -7374,18 +7327,14 @@
         <v>391</v>
       </c>
       <c r="C17" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D17" s="8">
         <v>1</v>
       </c>
-      <c r="F17" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(20, 3, 'InfoSecControls', b'1'),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>20</v>
       </c>
@@ -7393,245 +7342,224 @@
         <v>392</v>
       </c>
       <c r="C18" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>20</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="C19" s="8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D19" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>0</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="C20" s="8">
+        <v>30</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <f>A18+10</f>
+        <v>30</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="C21" s="8">
+        <v>1</v>
+      </c>
+      <c r="D21" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>30</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C22" s="8">
+        <f>C21+1</f>
+        <v>2</v>
+      </c>
+      <c r="D22" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>30</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C23" s="8">
+        <f t="shared" ref="C23:C26" si="1">C22+1</f>
+        <v>3</v>
+      </c>
+      <c r="D23" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>30</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C24" s="8">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="D18" s="8">
-        <v>1</v>
-      </c>
-      <c r="F18" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(20, 4, 'PictureMaker', b'1'),</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="D24" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>30</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="C25" s="8">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D25" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>30</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C26" s="8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D26" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
         <v>0</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="C19" s="8">
-        <v>30</v>
-      </c>
-      <c r="D19" s="8">
-        <v>1</v>
-      </c>
-      <c r="F19" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(0, 30, 'EventLog.Controllers', b'1'),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <f>A18+10</f>
-        <v>30</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="C20" s="8">
-        <v>1</v>
-      </c>
-      <c r="D20" s="8">
-        <v>1</v>
-      </c>
-      <c r="F20" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(30, 1, 'Utils.Authentication', b'1'),</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
-        <v>30</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="C21" s="8">
-        <f>C20+1</f>
-        <v>2</v>
-      </c>
-      <c r="D21" s="8">
-        <v>1</v>
-      </c>
-      <c r="F21" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(30, 2, 'Utils.Messaging', b'1'),</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
-        <v>30</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="C22" s="8">
-        <f t="shared" ref="C22:C24" si="4">C21+1</f>
-        <v>3</v>
-      </c>
-      <c r="D22" s="8">
-        <v>1</v>
-      </c>
-      <c r="F22" s="20" t="str">
-        <f t="shared" ref="F22" si="5">_xlfn.CONCAT("(",A22,", ",C22, ", '", B22, "', b'",D22,"'),")</f>
-        <v>(30, 3, 'Shared.EventLogs', b'1'),</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
-        <v>30</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="C23" s="8">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="D23" s="8">
-        <v>1</v>
-      </c>
-      <c r="F23" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(30, 4, 'InfoSecControls.SystemParameters', b'1'),</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
-        <v>30</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="C24" s="8">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="D24" s="8">
-        <v>1</v>
-      </c>
-      <c r="F24" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(30, 5, 'InfoSecControls.OrganizationPolicies', b'1'),</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
-        <v>0</v>
-      </c>
-      <c r="B25" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C27" s="8">
         <v>40</v>
       </c>
-      <c r="D25" s="8">
-        <v>1</v>
-      </c>
-      <c r="F25" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(0, 40, 'EventLog.Actions', b'1'),</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
-        <f>A24+10</f>
+      <c r="D27" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <f>A25+10</f>
         <v>40</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="C26" s="8">
-        <v>1</v>
-      </c>
-      <c r="D26" s="8">
-        <v>1</v>
-      </c>
-      <c r="F26" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(40, 1, 'Create', b'1'),</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
-        <v>40</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="C27" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="D27" s="8">
-        <v>1</v>
-      </c>
-      <c r="F27" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(40, 2, 'Read', b'1'),</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
-        <v>40</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>376</v>
-      </c>
       <c r="C28" s="8">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D28" s="8">
         <v>1</v>
       </c>
-      <c r="F28" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(40, 3, 'Update', b'1'),</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>40</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C29" s="8">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="D29" s="8">
         <v>1</v>
       </c>
-      <c r="F29" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>(40, 4, 'Delete', b'1'),</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>40</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="C30" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D30" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>40</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C31" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D31" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>40</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="C30" s="8">
-        <f t="shared" si="1"/>
+      <c r="C32" s="8">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D30" s="8">
-        <v>1</v>
-      </c>
-      <c r="F30" s="20" t="str">
-        <f t="shared" ref="F30" si="6">_xlfn.CONCAT("(",A30,", ",C30, ", '", B30, "', b'",D30,"'),")</f>
-        <v>(40, 5, 'List', b'1'),</v>
+      <c r="D32" s="8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B29" xr:uid="{AD08FBCA-206E-41A1-8589-5F1F7EE43364}"/>
+  <autoFilter ref="A1:B31" xr:uid="{AD08FBCA-206E-41A1-8589-5F1F7EE43364}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>